<commit_message>
created cytokine script and deleted lots of old files
</commit_message>
<xml_diff>
--- a/data/processed/cytokines.xlsx
+++ b/data/processed/cytokines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaare/Github/matrinem/data/processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdt/Documents/GitHub/2022_matrinem_thesis/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BD417D-655A-9D42-9507-9A885D752CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A92D497-DA4C-D54B-AAD4-9AEC93FB7C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,13 +191,13 @@
     <t>GENTA-FF</t>
   </si>
   <si>
-    <t>VANCO-FORM+FVT</t>
+    <t>group</t>
   </si>
   <si>
-    <t>VANCO-FORM+SM</t>
+    <t>VANCO-FVF</t>
   </si>
   <si>
-    <t>group</t>
+    <t>VANCO-SM</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D52C75A-9A6C-6949-8578-20A446AF8D59}">
   <dimension ref="A1:R144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -553,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -6954,7 +6954,7 @@
         <v>23</v>
       </c>
       <c r="D119" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E119" t="s">
         <v>51</v>
@@ -7010,7 +7010,7 @@
         <v>23</v>
       </c>
       <c r="D120" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E120" t="s">
         <v>51</v>
@@ -7066,7 +7066,7 @@
         <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E121" t="s">
         <v>51</v>
@@ -7122,7 +7122,7 @@
         <v>23</v>
       </c>
       <c r="D122" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E122" t="s">
         <v>51</v>
@@ -7178,7 +7178,7 @@
         <v>23</v>
       </c>
       <c r="D123" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E123" t="s">
         <v>51</v>
@@ -7234,7 +7234,7 @@
         <v>23</v>
       </c>
       <c r="D124" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E124" t="s">
         <v>51</v>
@@ -7290,7 +7290,7 @@
         <v>23</v>
       </c>
       <c r="D125" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E125" t="s">
         <v>51</v>
@@ -7346,7 +7346,7 @@
         <v>23</v>
       </c>
       <c r="D126" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E126" t="s">
         <v>51</v>
@@ -7402,7 +7402,7 @@
         <v>23</v>
       </c>
       <c r="D127" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E127" t="s">
         <v>51</v>
@@ -7458,7 +7458,7 @@
         <v>23</v>
       </c>
       <c r="D128" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E128" t="s">
         <v>51</v>
@@ -7514,7 +7514,7 @@
         <v>23</v>
       </c>
       <c r="D129" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E129" t="s">
         <v>51</v>
@@ -7570,7 +7570,7 @@
         <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E130" t="s">
         <v>51</v>
@@ -7626,7 +7626,7 @@
         <v>23</v>
       </c>
       <c r="D131" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E131" t="s">
         <v>51</v>
@@ -7682,7 +7682,7 @@
         <v>23</v>
       </c>
       <c r="D132" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E132" t="s">
         <v>51</v>
@@ -7738,7 +7738,7 @@
         <v>23</v>
       </c>
       <c r="D133" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E133" t="s">
         <v>51</v>
@@ -7794,7 +7794,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E134" t="s">
         <v>51</v>
@@ -7850,7 +7850,7 @@
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E135" t="s">
         <v>51</v>

</xml_diff>